<commit_message>
data wrangling part 1
</commit_message>
<xml_diff>
--- a/input/disaster_data/cyclone damages.xlsx
+++ b/input/disaster_data/cyclone damages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Dropbox\PhD thesis\chapitre_2\PhD-Chapter-2\input\disaster_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81729C96-02DD-4F04-8D7B-74E187229CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C28E26-2104-433F-B578-481FF3CF2D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="8880" activeTab="3" xr2:uid="{5F13E456-37DE-4CDC-BD39-2FDC878B176F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5F13E456-37DE-4CDC-BD39-2FDC878B176F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sidr" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,11 @@
     <sheet name="Roanu" sheetId="4" r:id="rId3"/>
     <sheet name="Komen" sheetId="5" r:id="rId4"/>
     <sheet name="Mora" sheetId="6" r:id="rId5"/>
-    <sheet name="source" sheetId="2" r:id="rId6"/>
+    <sheet name="total" sheetId="7" r:id="rId6"/>
+    <sheet name="source" sheetId="2" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="113">
   <si>
     <t>Government of Bangladesh Report (2008), “Cyclone Sidr in Bangladesh: Damage, Loss and Needs Assessment for Disaster Recovery and Reconstruction.https://reliefweb.int/sites/reliefweb.int/files/resources/F2FDFF067EF49C8DC12574DC00455142-Full_Report.pdf</t>
   </si>
@@ -365,6 +366,27 @@
   </si>
   <si>
     <t>Parbattya Chattagram</t>
+  </si>
+  <si>
+    <t>Affected people Komen</t>
+  </si>
+  <si>
+    <t>Affected people Roanu</t>
+  </si>
+  <si>
+    <t>Affected people Mora</t>
+  </si>
+  <si>
+    <t>Total affected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">District </t>
+  </si>
+  <si>
+    <t>Aff. hh.</t>
+  </si>
+  <si>
+    <t>Aff. P.</t>
   </si>
 </sst>
 </file>
@@ -434,7 +456,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -457,11 +479,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -525,6 +556,24 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5387,10 +5436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7617B3E-1E73-42CB-A895-5346D2DE721E}">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -5398,9 +5447,10 @@
     <col min="1" max="10" width="11.5546875" style="19"/>
     <col min="11" max="11" width="13.88671875" style="19" customWidth="1"/>
     <col min="12" max="15" width="11.5546875" style="19"/>
+    <col min="16" max="16" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="16" customFormat="1" ht="43.2">
+    <row r="1" spans="1:20" s="16" customFormat="1" ht="43.2">
       <c r="A1" s="17" t="s">
         <v>70</v>
       </c>
@@ -5446,8 +5496,23 @@
       <c r="O1" s="18" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q1" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" s="21" t="s">
         <v>30</v>
       </c>
@@ -5497,8 +5562,23 @@
       <c r="O2" s="19">
         <v>59595</v>
       </c>
-    </row>
-    <row r="3" spans="1:15">
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2">
+        <v>55625</v>
+      </c>
+      <c r="R2">
+        <v>80114</v>
+      </c>
+      <c r="S2">
+        <v>315060</v>
+      </c>
+      <c r="T2">
+        <v>478355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="21" t="s">
         <v>14</v>
       </c>
@@ -5548,8 +5628,20 @@
       <c r="O3" s="19">
         <v>29655</v>
       </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3">
+        <v>115908</v>
+      </c>
+      <c r="S3" t="s">
+        <v>103</v>
+      </c>
+      <c r="T3">
+        <v>463632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="21" t="s">
         <v>28</v>
       </c>
@@ -5599,8 +5691,23 @@
       <c r="O4" s="19">
         <v>3275</v>
       </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="P4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q4">
+        <v>7400</v>
+      </c>
+      <c r="R4">
+        <v>21914</v>
+      </c>
+      <c r="S4">
+        <v>38000</v>
+      </c>
+      <c r="T4">
+        <v>114765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
@@ -5650,8 +5757,23 @@
       <c r="O5" s="19">
         <v>411</v>
       </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5">
+        <v>20</v>
+      </c>
+      <c r="R5">
+        <v>420</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+      <c r="T5">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
@@ -5701,8 +5823,20 @@
       <c r="O6" s="19">
         <v>55</v>
       </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="P6" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6">
+        <v>70</v>
+      </c>
+      <c r="R6">
+        <v>203</v>
+      </c>
+      <c r="T6">
+        <v>262547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="21" t="s">
         <v>13</v>
       </c>
@@ -5752,8 +5886,23 @@
       <c r="O7" s="19">
         <v>2047</v>
       </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q7">
+        <v>238</v>
+      </c>
+      <c r="R7">
+        <v>18618</v>
+      </c>
+      <c r="S7">
+        <v>1175</v>
+      </c>
+      <c r="T7">
+        <v>88050</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="21" t="s">
         <v>3</v>
       </c>
@@ -5803,8 +5952,17 @@
       <c r="O8" s="19">
         <v>18315</v>
       </c>
-    </row>
-    <row r="9" spans="1:15">
+      <c r="P8" t="s">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>18315</v>
+      </c>
+      <c r="T8">
+        <v>73260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="21" t="s">
         <v>4</v>
       </c>
@@ -5854,8 +6012,20 @@
       <c r="O9" s="19">
         <v>6511</v>
       </c>
-    </row>
-    <row r="10" spans="1:15">
+      <c r="P9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>2009</v>
+      </c>
+      <c r="R9">
+        <v>6466</v>
+      </c>
+      <c r="T9">
+        <v>25864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="21" t="s">
         <v>9</v>
       </c>
@@ -5905,8 +6075,17 @@
       <c r="O10" s="19">
         <v>1500</v>
       </c>
-    </row>
-    <row r="11" spans="1:15">
+      <c r="P10" t="s">
+        <v>9</v>
+      </c>
+      <c r="R10">
+        <v>2000</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="21" t="s">
         <v>10</v>
       </c>
@@ -5956,8 +6135,23 @@
       <c r="O11" s="19">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:15">
+      <c r="P11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11">
+        <v>7000</v>
+      </c>
+      <c r="R11">
+        <v>7520</v>
+      </c>
+      <c r="S11">
+        <v>28000</v>
+      </c>
+      <c r="T11">
+        <v>30080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="21" t="s">
         <v>7</v>
       </c>
@@ -6006,6 +6200,15 @@
       </c>
       <c r="O12" s="19">
         <v>120</v>
+      </c>
+      <c r="P12" t="s">
+        <v>7</v>
+      </c>
+      <c r="R12">
+        <v>1100</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6016,15 +6219,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{413E47C0-D118-4437-9E4A-DE4F997F730E}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="43.2">
       <c r="A1" s="17" t="s">
         <v>70</v>
       </c>
@@ -6046,8 +6249,17 @@
       <c r="G1" s="18" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="J1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" s="27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
@@ -6055,7 +6267,7 @@
         <f>VLOOKUP(A2,Sidr!A:C,2,FALSE)</f>
         <v>Cox's Bazar</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="22">
         <f>VLOOKUP(A2,Sidr!A:C,3,FALSE)</f>
         <v>212</v>
       </c>
@@ -6071,8 +6283,17 @@
       <c r="G2">
         <v>84500</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>249412</v>
+      </c>
+      <c r="L2">
+        <v>1185675</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
@@ -6080,7 +6301,7 @@
         <f>VLOOKUP(A3,Sidr!A:C,2,FALSE)</f>
         <v>Chittagong</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="22">
         <f>VLOOKUP(A3,Sidr!A:C,3,FALSE)</f>
         <v>210</v>
       </c>
@@ -6096,8 +6317,17 @@
       <c r="G3">
         <v>1775</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>28820</v>
+      </c>
+      <c r="L3">
+        <v>144100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
@@ -6105,7 +6335,7 @@
         <f>VLOOKUP(A4,Sidr!A:C,2,FALSE)</f>
         <v>Noakhali</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="22">
         <f>VLOOKUP(A4,Sidr!A:C,3,FALSE)</f>
         <v>216</v>
       </c>
@@ -6121,8 +6351,17 @@
       <c r="G4">
         <v>1385</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="J4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4">
+        <v>30000</v>
+      </c>
+      <c r="L4">
+        <v>150000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="13" t="s">
         <v>18</v>
       </c>
@@ -6130,7 +6369,7 @@
         <f>VLOOKUP(A5,Sidr!A:C,2,FALSE)</f>
         <v>Feni</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="22">
         <f>VLOOKUP(A5,Sidr!A:C,3,FALSE)</f>
         <v>213</v>
       </c>
@@ -6146,15 +6385,24 @@
       <c r="G5">
         <v>2052</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>21132</v>
+      </c>
+      <c r="L5">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="15" t="s">
         <v>87</v>
       </c>
       <c r="B6" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="10" t="str">
+      <c r="C6" s="22" t="str">
         <f>VLOOKUP(B6,[1]Sheet1!$H:$L,2,FALSE)</f>
         <v>27</v>
       </c>
@@ -6169,6 +6417,15 @@
       </c>
       <c r="G6">
         <v>5752</v>
+      </c>
+      <c r="J6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6">
+        <v>17025</v>
+      </c>
+      <c r="L6">
+        <v>63167</v>
       </c>
     </row>
   </sheetData>
@@ -6178,15 +6435,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04E099BD-C32C-4FC5-9153-14EFC6E49CA8}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" s="11" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="57.6">
       <c r="A1" s="17" t="s">
         <v>70</v>
       </c>
@@ -6208,8 +6465,17 @@
       <c r="G1" s="18" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="J1" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="13" t="s">
         <v>30</v>
       </c>
@@ -6217,7 +6483,7 @@
         <f>VLOOKUP(A2,Sidr!A:C,2,FALSE)</f>
         <v>Cox's Bazar</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="22">
         <f>VLOOKUP(A2,Sidr!A:C,3,FALSE)</f>
         <v>212</v>
       </c>
@@ -6237,8 +6503,17 @@
         <f>F2*5</f>
         <v>227800</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2">
+        <v>15443</v>
+      </c>
+      <c r="L2">
+        <v>227800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="13" t="s">
         <v>14</v>
       </c>
@@ -6246,7 +6521,7 @@
         <f>VLOOKUP(A3,Sidr!A:C,2,FALSE)</f>
         <v>Chittagong</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="22">
         <f>VLOOKUP(A3,Sidr!A:C,3,FALSE)</f>
         <v>210</v>
       </c>
@@ -6266,15 +6541,24 @@
         <f t="shared" ref="G3:G5" si="0">F3*5</f>
         <v>27555</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="22.8">
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>2765</v>
+      </c>
+      <c r="L3">
+        <v>27555</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="22.8">
       <c r="A4" s="13" t="s">
         <v>94</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="C4" s="22" t="str">
         <f>VLOOKUP(B4,[1]Sheet1!$H:$L,2,FALSE)</f>
         <v>217</v>
       </c>
@@ -6292,15 +6576,24 @@
         <f t="shared" si="0"/>
         <v>5885</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="J4" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4">
+        <v>150</v>
+      </c>
+      <c r="L4">
+        <v>5885</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="15" t="s">
         <v>87</v>
       </c>
       <c r="B5" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="10" t="str">
+      <c r="C5" s="22" t="str">
         <f>VLOOKUP(B5,[1]Sheet1!$H:$L,2,FALSE)</f>
         <v>27</v>
       </c>
@@ -6316,6 +6609,15 @@
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
+        <v>14250</v>
+      </c>
+      <c r="J5" t="s">
+        <v>104</v>
+      </c>
+      <c r="K5">
+        <v>850</v>
+      </c>
+      <c r="L5">
         <v>14250</v>
       </c>
     </row>
@@ -6325,6 +6627,403 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDD8DE6-857D-4F28-9F69-7FD402352B48}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="5" max="5" width="14.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="43.2">
+      <c r="A1" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="22" t="str">
+        <f>VLOOKUP(A2,Sidr!A:C,2,FALSE)</f>
+        <v>Cox's Bazar</v>
+      </c>
+      <c r="C2" s="22">
+        <f>VLOOKUP(A2,Sidr!A:C,3,FALSE)</f>
+        <v>212</v>
+      </c>
+      <c r="D2">
+        <f>VLOOKUP(A2,Komen!A:E,5,FALSE)</f>
+        <v>1185675</v>
+      </c>
+      <c r="E2">
+        <f>VLOOKUP(A2,Roanu!A:M,13,FALSE)</f>
+        <v>478355</v>
+      </c>
+      <c r="F2">
+        <f>VLOOKUP(A2,Mora!A:G,7,FALSE)</f>
+        <v>227800</v>
+      </c>
+      <c r="G2">
+        <f>SUM(D2:F2)</f>
+        <v>1891830</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="22" t="str">
+        <f>VLOOKUP(A3,Sidr!A:C,2,FALSE)</f>
+        <v>Chittagong</v>
+      </c>
+      <c r="C3" s="22">
+        <f>VLOOKUP(A3,Sidr!A:C,3,FALSE)</f>
+        <v>210</v>
+      </c>
+      <c r="D3">
+        <f>VLOOKUP(A3,Komen!A:E,5,FALSE)</f>
+        <v>144100</v>
+      </c>
+      <c r="E3">
+        <f>VLOOKUP(A3,Roanu!A:M,13,FALSE)</f>
+        <v>463632</v>
+      </c>
+      <c r="F3">
+        <f>VLOOKUP(A3,Mora!A:G,7,FALSE)</f>
+        <v>27555</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G14" si="0">SUM(D3:F3)</f>
+        <v>635287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="22" t="str">
+        <f>VLOOKUP(A4,Sidr!A:C,2,FALSE)</f>
+        <v>Noakhali</v>
+      </c>
+      <c r="C4" s="22">
+        <f>VLOOKUP(A4,Sidr!A:C,3,FALSE)</f>
+        <v>216</v>
+      </c>
+      <c r="D4">
+        <f>VLOOKUP(A4,Komen!A:E,5,FALSE)</f>
+        <v>150000</v>
+      </c>
+      <c r="E4">
+        <f>VLOOKUP(A4,Roanu!A:M,13,FALSE)</f>
+        <v>114765</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <f>SUM(D4:F4)</f>
+        <v>264765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="22" t="str">
+        <f>VLOOKUP(A5,Sidr!A:C,2,FALSE)</f>
+        <v>Lakshmipur</v>
+      </c>
+      <c r="C5" s="22">
+        <f>VLOOKUP(A5,Sidr!A:C,3,FALSE)</f>
+        <v>215</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>VLOOKUP(A5,Roanu!A:M,13,FALSE)</f>
+        <v>1700</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="22" t="str">
+        <f>VLOOKUP(A6,Sidr!A:C,2,FALSE)</f>
+        <v>Feni</v>
+      </c>
+      <c r="C6" s="22">
+        <f>VLOOKUP(A6,Sidr!A:C,3,FALSE)</f>
+        <v>213</v>
+      </c>
+      <c r="D6">
+        <f>VLOOKUP(A6,Komen!A:E,5,FALSE)</f>
+        <v>42000</v>
+      </c>
+      <c r="E6">
+        <f>VLOOKUP(A6,Roanu!A:M,13,FALSE)</f>
+        <v>262547</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>304547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="22" t="str">
+        <f>VLOOKUP(A7,Sidr!A:C,2,FALSE)</f>
+        <v>Chandpur</v>
+      </c>
+      <c r="C7" s="22">
+        <f>VLOOKUP(A7,Sidr!A:C,3,FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>VLOOKUP(A7,Roanu!A:M,13,FALSE)</f>
+        <v>88050</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>88050</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="22" t="str">
+        <f>VLOOKUP(A8,Sidr!A:C,2,FALSE)</f>
+        <v>Barisal</v>
+      </c>
+      <c r="C8" s="22">
+        <f>VLOOKUP(A8,Sidr!A:C,3,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f>VLOOKUP(A8,Roanu!A:M,13,FALSE)</f>
+        <v>73260</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>73260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="22" t="str">
+        <f>VLOOKUP(A9,Sidr!A:C,2,FALSE)</f>
+        <v>Bhola</v>
+      </c>
+      <c r="C9" s="22">
+        <f>VLOOKUP(A9,Sidr!A:C,3,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>VLOOKUP(A9,Roanu!A:M,13,FALSE)</f>
+        <v>25864</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>25864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="22" t="str">
+        <f>VLOOKUP(A10,Sidr!A:C,2,FALSE)</f>
+        <v>Patuakhali</v>
+      </c>
+      <c r="C10" s="22">
+        <f>VLOOKUP(A10,Sidr!A:C,3,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>VLOOKUP(A10,Roanu!A:M,13,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="str">
+        <f>VLOOKUP(A11,Sidr!A:C,2,FALSE)</f>
+        <v>Pirojpur</v>
+      </c>
+      <c r="C11" s="22">
+        <f>VLOOKUP(A11,Sidr!A:C,3,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f>VLOOKUP(A11,Roanu!A:M,13,FALSE)</f>
+        <v>30080</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>30080</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="22" t="str">
+        <f>VLOOKUP(A12,Sidr!A:C,2,FALSE)</f>
+        <v>Khulna</v>
+      </c>
+      <c r="C12" s="22">
+        <f>VLOOKUP(A12,Sidr!A:C,3,FALSE)</f>
+        <v>439</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>VLOOKUP(A12,Roanu!A:M,13,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>SUM(D12:F12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C13" s="22" t="str">
+        <f>VLOOKUP(B13,[1]Sheet1!$H:$L,2,FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>63167</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f>VLOOKUP(A13,Mora!A:G,7,FALSE)</f>
+        <v>14250</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>77417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="22.8">
+      <c r="A14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="22" t="str">
+        <f>VLOOKUP(B14,[1]Sheet1!$H:$L,2,FALSE)</f>
+        <v>217</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f>VLOOKUP(A14,Mora!A:G,7,FALSE)</f>
+        <v>5885</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>5885</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{715F4B6D-1853-4BA4-B23C-510566FF409F}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>